<commit_message>
update description for SIC87
</commit_message>
<xml_diff>
--- a/data-raw/sic.decs.raw.xlsx
+++ b/data-raw/sic.decs.raw.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siqichen/Documents/GitHub/concordance/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siqichen/phd UCR/summer job/23 GSR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827BF71A-6222-214A-8635-E0D96B907972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C288D79-5B2A-A24A-B404-091BC3A25EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{D6F1DE26-8682-4842-A87D-7811FDF6DFE0}"/>
   </bookViews>
@@ -5712,27 +5712,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>des2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>des3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>des4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>digits2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>digits3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>digits4</t>
+    <t>digit2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>digit3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>digit4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6127,29 +6127,29 @@
   <dimension ref="A1:F1190"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1803</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1804</v>
       </c>
-      <c r="B1" t="s">
-        <v>1801</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1805</v>
       </c>
-      <c r="D1" t="s">
-        <v>1802</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1806</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1803</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>